<commit_message>
Final Work for 12/12
</commit_message>
<xml_diff>
--- a/JobSearch Relationships.xlsx
+++ b/JobSearch Relationships.xlsx
@@ -67,7 +67,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +85,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -171,17 +179,27 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +504,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,118 +514,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9" t="s">
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9" t="s">
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9" t="s">
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
     </row>
     <row r="4" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="5"/>
@@ -630,7 +648,7 @@
       <c r="S4" s="4"/>
     </row>
     <row r="5" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4"/>
@@ -639,7 +657,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="10"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="7"/>
       <c r="J5" s="2"/>
       <c r="K5" s="1"/>
@@ -653,7 +671,7 @@
       <c r="S5" s="4"/>
     </row>
     <row r="6" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="4"/>
@@ -676,7 +694,7 @@
       <c r="S6" s="4"/>
     </row>
     <row r="7" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="4"/>
@@ -699,7 +717,7 @@
       <c r="S7" s="4"/>
     </row>
     <row r="8" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="6"/>
@@ -722,7 +740,7 @@
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="4"/>
@@ -749,54 +767,54 @@
         <v>10</v>
       </c>
       <c r="K11" s="14"/>
-      <c r="L11" s="12"/>
+      <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="12"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K13" s="5"/>
-      <c r="L13" s="12"/>
+      <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J14" s="13" t="s">
+      <c r="J14" s="12" t="s">
         <v>12</v>
       </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="12"/>
+      <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J15" s="13" t="s">
+      <c r="J15" s="12" t="s">
         <v>13</v>
       </c>
       <c r="K15" s="3"/>
-      <c r="L15" s="12"/>
+      <c r="L15" s="11"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="12" t="s">
         <v>14</v>
       </c>
       <c r="K16" s="7"/>
-      <c r="L16" s="12"/>
+      <c r="L16" s="11"/>
     </row>
     <row r="17" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
     </row>
     <row r="18" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
     </row>
     <row r="19" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>